<commit_message>
created new framework for capita
</commit_message>
<xml_diff>
--- a/contactData.xlsx
+++ b/contactData.xlsx
@@ -1,25 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FDA712-90BD-48A9-A4F0-C6F17690BDAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>FirstName</t>
   </si>
@@ -117,13 +111,16 @@
   </si>
   <si>
     <t>data</t>
+  </si>
+  <si>
+    <t>Roshan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,7 +252,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -290,7 +287,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -467,21 +464,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -489,7 +486,7 @@
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -503,7 +500,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="5" customFormat="1">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -517,9 +514,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -531,7 +528,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -545,7 +542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -565,14 +562,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{538663AB-A25F-467A-8D06-3617FA408C03}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
@@ -580,7 +577,7 @@
     <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -594,7 +591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -608,7 +605,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -622,7 +619,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>21</v>
       </c>
@@ -636,7 +633,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -656,16 +653,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E1975A-BC74-4413-9878-5A8CC4059D2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>1</v>
       </c>
@@ -676,7 +673,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>4</v>
       </c>
@@ -687,7 +684,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="6" t="s">
         <v>29</v>
       </c>
@@ -695,7 +692,7 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -709,7 +706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="5" t="s">
         <v>4</v>
       </c>
@@ -723,7 +720,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -737,7 +734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -751,7 +748,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>

</xml_diff>